<commit_message>
docs: se actualiza calculo de recursos
</commit_message>
<xml_diff>
--- a/Segundo periodo/Informe de costos/CALCULO DE RECURSOS MAE MARKET.xlsx
+++ b/Segundo periodo/Informe de costos/CALCULO DE RECURSOS MAE MARKET.xlsx
@@ -1,23 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24430"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\palis\OneDrive\Escritorio\PROYECTO MAE MARKET- 26 ABRIL\Segundo Trimestre\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF36C955-C19F-45AC-A35E-9901D375524E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11490" windowHeight="4560"/>
+    <workbookView xWindow="2295" yWindow="2295" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="T-R-H" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -92,10 +102,10 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;\ * #,##0_);_(&quot;$&quot;\ * \(#,##0\);_(&quot;$&quot;\ * &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="_([$$-240A]\ * #,##0_);_([$$-240A]\ * \(#,##0\);_([$$-240A]\ * &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(&quot;$&quot;\ * #,##0_);_(&quot;$&quot;\ * \(#,##0\);_(&quot;$&quot;\ * &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="_([$$-240A]\ * #,##0_);_([$$-240A]\ * \(#,##0\);_([$$-240A]\ * &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -249,15 +259,6 @@
   </cellStyleXfs>
   <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -267,14 +268,47 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -284,37 +318,13 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -603,11 +613,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -618,208 +628,208 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18.75" x14ac:dyDescent="0.4">
-      <c r="A1" s="1"/>
-      <c r="B1" s="11" t="s">
+      <c r="A1" s="22"/>
+      <c r="B1" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
     </row>
     <row r="2" spans="1:6" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3"/>
-      <c r="B2" s="12" t="s">
+      <c r="A2" s="23"/>
+      <c r="B2" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="16" t="s">
+      <c r="D2" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="3"/>
-      <c r="B3" s="13"/>
-      <c r="C3" s="13"/>
-      <c r="D3" s="14" t="s">
+      <c r="A3" s="23"/>
+      <c r="B3" s="21"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="14" t="s">
+      <c r="E3" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="F3" s="14" t="s">
+      <c r="F3" s="8" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
-      <c r="B4" s="5" t="s">
+      <c r="A4" s="24"/>
+      <c r="B4" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="7">
+      <c r="C4" s="4">
         <v>908526</v>
       </c>
-      <c r="D4" s="7">
+      <c r="D4" s="4">
         <v>908526</v>
       </c>
-      <c r="E4" s="7">
-        <f>D4/22</f>
-        <v>41296.63636363636</v>
-      </c>
-      <c r="F4" s="7">
-        <f>E4/6</f>
-        <v>6882.772727272727</v>
+      <c r="E4" s="4">
+        <f>D4/30</f>
+        <v>30284.2</v>
+      </c>
+      <c r="F4" s="4">
+        <f>E4/8</f>
+        <v>3785.5250000000001</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="15" t="s">
+      <c r="A5" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="8">
+      <c r="C5" s="5">
         <v>2500000</v>
       </c>
-      <c r="D5" s="8">
+      <c r="D5" s="5">
         <f>C5/36</f>
         <v>69444.444444444438</v>
       </c>
-      <c r="E5" s="9">
+      <c r="E5" s="6">
         <f>D5/22</f>
         <v>3156.5656565656564</v>
       </c>
-      <c r="F5" s="8">
+      <c r="F5" s="5">
         <f>E5/6</f>
         <v>526.0942760942761</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="16" t="s">
+      <c r="A6" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="7">
+      <c r="C6" s="4">
         <v>0</v>
       </c>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+      <c r="F6" s="7"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="16"/>
-      <c r="B7" s="5" t="s">
+      <c r="A7" s="18"/>
+      <c r="B7" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="7">
+      <c r="C7" s="4">
         <v>0</v>
       </c>
-      <c r="D7" s="10"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="10"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
+      <c r="F7" s="7"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="16"/>
-      <c r="B8" s="5" t="s">
+      <c r="A8" s="18"/>
+      <c r="B8" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="7">
+      <c r="C8" s="4">
         <v>0</v>
       </c>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="10"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="7"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="16"/>
-      <c r="B9" s="5" t="s">
+      <c r="A9" s="18"/>
+      <c r="B9" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="7">
+      <c r="C9" s="4">
         <v>0</v>
       </c>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="10"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7"/>
+      <c r="F9" s="7"/>
     </row>
     <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="16"/>
-      <c r="B10" s="17" t="s">
+      <c r="A10" s="18"/>
+      <c r="B10" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="7">
+      <c r="C10" s="4">
         <f>E16</f>
         <v>347400</v>
       </c>
-      <c r="D10" s="10"/>
-      <c r="E10" s="10"/>
-      <c r="F10" s="10"/>
+      <c r="D10" s="7"/>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B13" s="4"/>
-      <c r="C13" s="23" t="s">
+      <c r="B13" s="1"/>
+      <c r="C13" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="D13" s="24" t="s">
+      <c r="D13" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="E13" s="24"/>
+      <c r="E13" s="14"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B14" s="23" t="s">
+      <c r="B14" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="C14" s="20">
+      <c r="C14" s="11">
         <v>73000</v>
       </c>
-      <c r="D14" s="21">
+      <c r="D14" s="15">
         <f>C14*3</f>
         <v>219000</v>
       </c>
-      <c r="E14" s="21"/>
+      <c r="E14" s="15"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B15" s="23" t="s">
+      <c r="B15" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="C15" s="20">
+      <c r="C15" s="11">
         <v>42800</v>
       </c>
-      <c r="D15" s="21">
+      <c r="D15" s="15">
         <f>C15*3</f>
         <v>128400</v>
       </c>
-      <c r="E15" s="21"/>
+      <c r="E15" s="15"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B16" s="18"/>
-      <c r="C16" s="19"/>
-      <c r="D16" s="14" t="s">
+      <c r="B16" s="16"/>
+      <c r="C16" s="17"/>
+      <c r="D16" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="E16" s="22">
+      <c r="E16" s="12">
         <f>D14+D15</f>
         <v>347400</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="A1:A4"/>
     <mergeCell ref="D13:E13"/>
     <mergeCell ref="D14:E14"/>
     <mergeCell ref="D15:E15"/>
     <mergeCell ref="B16:C16"/>
     <mergeCell ref="A6:A10"/>
-    <mergeCell ref="D2:F2"/>
-    <mergeCell ref="B1:F1"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="A1:A4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>